<commit_message>
feat(xlsx, league): export all files as single sheet, add league_season_details.py, minor changes
</commit_message>
<xml_diff>
--- a/data/countries.xlsx
+++ b/data/countries.xlsx
@@ -7,7 +7,7 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="countries" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
@@ -1849,7 +1849,7 @@
         <v>0</v>
       </c>
       <c r="E4">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="F4" t="s">
         <v>463</v>
@@ -1969,7 +1969,7 @@
         <v>41</v>
       </c>
       <c r="E10">
-        <v>5224</v>
+        <v>5225</v>
       </c>
       <c r="F10" t="s">
         <v>463</v>
@@ -3283,7 +3283,7 @@
         <v>756</v>
       </c>
       <c r="E76">
-        <v>16578</v>
+        <v>16577</v>
       </c>
       <c r="F76" t="s">
         <v>463</v>
@@ -3857,7 +3857,7 @@
         <v>0</v>
       </c>
       <c r="E105">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="F105" t="s">
         <v>463</v>
@@ -4437,7 +4437,7 @@
         <v>29</v>
       </c>
       <c r="E134">
-        <v>2513</v>
+        <v>2514</v>
       </c>
       <c r="F134" t="s">
         <v>463</v>
@@ -6028,7 +6028,7 @@
         <v>289</v>
       </c>
       <c r="E214">
-        <v>7107</v>
+        <v>7106</v>
       </c>
       <c r="F214" t="s">
         <v>463</v>

</xml_diff>